<commit_message>
WIP still some bugs
</commit_message>
<xml_diff>
--- a/touches liste.xlsx
+++ b/touches liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VincentBenet\Documents\GITHUB_VINCENTBENET\keyboard_steamdeck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9A1ADE-B686-40E1-844F-6D4C7C3DAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AE8A76-E727-4E60-9E7B-8A9E410A3BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{925326E3-CF88-4988-8F56-E8183DB2C6D0}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{925326E3-CF88-4988-8F56-E8183DB2C6D0}"/>
   </bookViews>
   <sheets>
     <sheet name="KEYS" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="627">
   <si>
     <t>CODE</t>
   </si>
@@ -1373,42 +1373,15 @@
     <t>=</t>
   </si>
   <si>
-    <t>Stop</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t>Help</t>
-  </si>
-  <si>
-    <t>Execute</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
-    <t>&lt;</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
     <t>&amp;</t>
   </si>
   <si>
-    <t>&amp;&amp;</t>
-  </si>
-  <si>
     <t>|</t>
   </si>
   <si>
-    <t>||</t>
-  </si>
-  <si>
     <t>:</t>
   </si>
   <si>
@@ -1421,9 +1394,6 @@
     <t>!</t>
   </si>
   <si>
-    <t>Space</t>
-  </si>
-  <si>
     <t>^</t>
   </si>
   <si>
@@ -1454,42 +1424,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>F13</t>
-  </si>
-  <si>
-    <t>F14</t>
-  </si>
-  <si>
-    <t>F15</t>
-  </si>
-  <si>
-    <t>F16</t>
-  </si>
-  <si>
-    <t>F17</t>
-  </si>
-  <si>
-    <t>F18</t>
-  </si>
-  <si>
-    <t>F19</t>
-  </si>
-  <si>
-    <t>F20</t>
-  </si>
-  <si>
-    <t>F21</t>
-  </si>
-  <si>
-    <t>F22</t>
-  </si>
-  <si>
-    <t>F23</t>
-  </si>
-  <si>
-    <t>F24</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -1565,37 +1499,7 @@
     <t>w</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>é</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>DELETE</t>
@@ -2043,7 +1947,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2086,6 +1990,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2345,7 +2256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2474,6 +2385,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2796,8 +2716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F67615D-6C6B-4545-830A-5005E3C48D17}">
   <dimension ref="A1:F251"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,19 +2735,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>531</v>
+        <v>499</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>532</v>
+        <v>500</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>433</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>480</v>
+        <v>458</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2835,10 +2755,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>603</v>
+        <v>571</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
       <c r="D2" s="40"/>
       <c r="E2" s="41"/>
@@ -2849,7 +2769,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>604</v>
+        <v>572</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>433</v>
@@ -2863,7 +2783,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>605</v>
+        <v>573</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>432</v>
@@ -2877,7 +2797,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>606</v>
+        <v>574</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>431</v>
@@ -2942,7 +2862,7 @@
         <v>221</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>476</v>
+        <v>454</v>
       </c>
       <c r="D10" s="40"/>
       <c r="E10" s="41"/>
@@ -2956,7 +2876,7 @@
         <v>226</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>481</v>
+        <v>459</v>
       </c>
       <c r="D11" s="40"/>
       <c r="E11" s="41"/>
@@ -2975,7 +2895,7 @@
       <c r="D12" s="40"/>
       <c r="E12" s="41"/>
       <c r="F12" s="44" t="s">
-        <v>540</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3000,11 +2920,11 @@
         <v>229</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>482</v>
+        <v>460</v>
       </c>
       <c r="D14" s="40"/>
       <c r="E14" s="41" t="s">
-        <v>521</v>
+        <v>489</v>
       </c>
       <c r="F14" s="43"/>
     </row>
@@ -3021,7 +2941,7 @@
       <c r="D15" s="40"/>
       <c r="E15" s="41"/>
       <c r="F15" s="44" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3032,7 +2952,7 @@
         <v>231</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>483</v>
+        <v>461</v>
       </c>
       <c r="D16" s="40"/>
       <c r="E16" s="41"/>
@@ -3046,7 +2966,7 @@
         <v>232</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>484</v>
+        <v>462</v>
       </c>
       <c r="D17" s="40"/>
       <c r="E17" s="41"/>
@@ -3060,7 +2980,7 @@
         <v>233</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="41"/>
@@ -3074,7 +2994,7 @@
         <v>234</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>486</v>
+        <v>464</v>
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="41"/>
@@ -3088,7 +3008,7 @@
         <v>235</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>487</v>
+        <v>465</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="41"/>
@@ -3102,7 +3022,7 @@
         <v>236</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>488</v>
+        <v>466</v>
       </c>
       <c r="D21" s="40"/>
       <c r="E21" s="41"/>
@@ -3119,7 +3039,7 @@
         <v>430</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>520</v>
+        <v>488</v>
       </c>
       <c r="E22" s="41"/>
       <c r="F22" s="43"/>
@@ -3132,7 +3052,7 @@
         <v>238</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>489</v>
+        <v>467</v>
       </c>
       <c r="D23" s="40"/>
       <c r="E23" s="41"/>
@@ -3146,7 +3066,7 @@
         <v>239</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="41"/>
@@ -3160,7 +3080,7 @@
         <v>240</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>491</v>
+        <v>469</v>
       </c>
       <c r="D25" s="40"/>
       <c r="E25" s="41"/>
@@ -3174,7 +3094,7 @@
         <v>241</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>492</v>
+        <v>470</v>
       </c>
       <c r="D26" s="40"/>
       <c r="E26" s="41"/>
@@ -3188,12 +3108,12 @@
         <v>242</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>493</v>
+        <v>471</v>
       </c>
       <c r="D27" s="40"/>
       <c r="E27" s="41"/>
       <c r="F27" s="43" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3204,7 +3124,7 @@
         <v>243</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
       <c r="D28" s="40"/>
       <c r="E28" s="41"/>
@@ -3218,7 +3138,7 @@
         <v>244</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="D29" s="40"/>
       <c r="E29" s="41"/>
@@ -3232,7 +3152,7 @@
         <v>245</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="D30" s="40"/>
       <c r="E30" s="41"/>
@@ -3251,7 +3171,7 @@
       <c r="D31" s="40"/>
       <c r="E31" s="41"/>
       <c r="F31" s="43" t="s">
-        <v>542</v>
+        <v>510</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3262,12 +3182,12 @@
         <v>247</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>497</v>
+        <v>475</v>
       </c>
       <c r="D32" s="40"/>
       <c r="E32" s="41"/>
       <c r="F32" s="44" t="s">
-        <v>563</v>
+        <v>531</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3278,12 +3198,12 @@
         <v>248</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="D33" s="40"/>
       <c r="E33" s="41"/>
       <c r="F33" s="44" t="s">
-        <v>541</v>
+        <v>509</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -3294,12 +3214,12 @@
         <v>249</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="D34" s="40"/>
       <c r="E34" s="41"/>
       <c r="F34" s="44" t="s">
-        <v>564</v>
+        <v>532</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -3310,12 +3230,12 @@
         <v>250</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="D35" s="40"/>
       <c r="E35" s="41"/>
       <c r="F35" s="44" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3326,7 +3246,7 @@
         <v>251</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="D36" s="40">
         <v>1</v>
@@ -3342,13 +3262,13 @@
         <v>252</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>504</v>
+        <v>479</v>
       </c>
       <c r="D37" s="40">
         <v>2</v>
       </c>
       <c r="E37" s="41" t="s">
-        <v>565</v>
+        <v>533</v>
       </c>
       <c r="F37" s="43"/>
     </row>
@@ -3360,13 +3280,13 @@
         <v>253</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>513</v>
+        <v>481</v>
       </c>
       <c r="D38" s="40">
         <v>3</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="F38" s="43"/>
     </row>
@@ -3378,13 +3298,13 @@
         <v>254</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>574</v>
+        <v>542</v>
       </c>
       <c r="D39" s="40">
         <v>4</v>
       </c>
       <c r="E39" s="41" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="F39" s="43"/>
     </row>
@@ -3396,13 +3316,13 @@
         <v>255</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="D40" s="40">
         <v>5</v>
       </c>
       <c r="E40" s="41" t="s">
-        <v>517</v>
+        <v>485</v>
       </c>
       <c r="F40" s="43"/>
     </row>
@@ -3414,13 +3334,13 @@
         <v>256</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="D41" s="40">
         <v>6</v>
       </c>
       <c r="E41" s="41" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="F41" s="43"/>
     </row>
@@ -3432,13 +3352,13 @@
         <v>257</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>514</v>
+        <v>482</v>
       </c>
       <c r="D42" s="40">
         <v>7</v>
       </c>
       <c r="E42" s="41" t="s">
-        <v>519</v>
+        <v>487</v>
       </c>
       <c r="F42" s="43"/>
     </row>
@@ -3450,13 +3370,13 @@
         <v>258</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>515</v>
+        <v>483</v>
       </c>
       <c r="D43" s="40">
         <v>8</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>518</v>
+        <v>486</v>
       </c>
       <c r="F43" s="43"/>
     </row>
@@ -3474,7 +3394,7 @@
         <v>9</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="F44" s="43"/>
     </row>
@@ -3486,13 +3406,13 @@
         <v>260</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>516</v>
+        <v>484</v>
       </c>
       <c r="D45" s="40">
         <v>0</v>
       </c>
       <c r="E45" s="41" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="F45" s="43"/>
     </row>
@@ -3532,7 +3452,7 @@
         <v>263</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>538</v>
+        <v>506</v>
       </c>
       <c r="D48" s="40"/>
       <c r="E48" s="41"/>
@@ -3546,7 +3466,7 @@
         <v>264</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>539</v>
+        <v>507</v>
       </c>
       <c r="D49" s="40"/>
       <c r="E49" s="41"/>
@@ -3560,7 +3480,7 @@
         <v>265</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>537</v>
+        <v>505</v>
       </c>
       <c r="D50" s="40"/>
       <c r="E50" s="41"/>
@@ -3574,13 +3494,13 @@
         <v>266</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>522</v>
+        <v>490</v>
       </c>
       <c r="E51" s="41" t="s">
-        <v>523</v>
+        <v>491</v>
       </c>
       <c r="F51" s="43"/>
     </row>
@@ -3595,10 +3515,10 @@
         <v>436</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="E52" s="41" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="F52" s="43"/>
     </row>
@@ -3610,10 +3530,10 @@
         <v>268</v>
       </c>
       <c r="C53" s="37" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>524</v>
+        <v>492</v>
       </c>
       <c r="E53" s="41"/>
       <c r="F53" s="43"/>
@@ -3626,13 +3546,13 @@
         <v>269</v>
       </c>
       <c r="C54" s="37" t="s">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="E54" s="41" t="s">
-        <v>525</v>
+        <v>493</v>
       </c>
       <c r="F54" s="43"/>
     </row>
@@ -3644,10 +3564,10 @@
         <v>270</v>
       </c>
       <c r="C55" s="37" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>526</v>
+        <v>494</v>
       </c>
       <c r="E55" s="41"/>
       <c r="F55" s="43"/>
@@ -3672,7 +3592,7 @@
         <v>272</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>527</v>
+        <v>495</v>
       </c>
       <c r="D57" s="40"/>
       <c r="E57" s="41"/>
@@ -3686,10 +3606,10 @@
         <v>273</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>529</v>
+        <v>497</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E58" s="41"/>
       <c r="F58" s="43"/>
@@ -3716,10 +3636,10 @@
         <v>275</v>
       </c>
       <c r="C60" s="37" t="s">
-        <v>479</v>
+        <v>457</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="E60" s="41"/>
       <c r="F60" s="43"/>
@@ -3732,9 +3652,11 @@
         <v>276</v>
       </c>
       <c r="C61" s="37" t="s">
+        <v>440</v>
+      </c>
+      <c r="D61" s="40" t="s">
         <v>449</v>
       </c>
-      <c r="D61" s="40"/>
       <c r="E61" s="41"/>
       <c r="F61" s="43"/>
     </row>
@@ -3746,10 +3668,10 @@
         <v>277</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>530</v>
+        <v>498</v>
       </c>
       <c r="E62" s="41"/>
       <c r="F62" s="43"/>
@@ -3776,7 +3698,7 @@
         <v>279</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>548</v>
+        <v>516</v>
       </c>
       <c r="D64" s="40"/>
       <c r="E64" s="41"/>
@@ -3790,7 +3712,7 @@
         <v>280</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>549</v>
+        <v>517</v>
       </c>
       <c r="D65" s="40"/>
       <c r="E65" s="41"/>
@@ -3804,7 +3726,7 @@
         <v>281</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>550</v>
+        <v>518</v>
       </c>
       <c r="D66" s="40"/>
       <c r="E66" s="41"/>
@@ -3818,7 +3740,7 @@
         <v>282</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>551</v>
+        <v>519</v>
       </c>
       <c r="D67" s="40"/>
       <c r="E67" s="41"/>
@@ -3832,7 +3754,7 @@
         <v>283</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>552</v>
+        <v>520</v>
       </c>
       <c r="D68" s="40"/>
       <c r="E68" s="41"/>
@@ -3846,7 +3768,7 @@
         <v>284</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>553</v>
+        <v>521</v>
       </c>
       <c r="D69" s="40"/>
       <c r="E69" s="41"/>
@@ -3860,7 +3782,7 @@
         <v>285</v>
       </c>
       <c r="C70" s="37" t="s">
-        <v>554</v>
+        <v>522</v>
       </c>
       <c r="D70" s="40"/>
       <c r="E70" s="41"/>
@@ -3874,7 +3796,7 @@
         <v>286</v>
       </c>
       <c r="C71" s="37" t="s">
-        <v>555</v>
+        <v>523</v>
       </c>
       <c r="D71" s="40"/>
       <c r="E71" s="41"/>
@@ -3888,7 +3810,7 @@
         <v>287</v>
       </c>
       <c r="C72" s="37" t="s">
-        <v>556</v>
+        <v>524</v>
       </c>
       <c r="D72" s="40"/>
       <c r="E72" s="41"/>
@@ -3902,7 +3824,7 @@
         <v>288</v>
       </c>
       <c r="C73" s="37" t="s">
-        <v>557</v>
+        <v>525</v>
       </c>
       <c r="D73" s="40"/>
       <c r="E73" s="41"/>
@@ -3916,7 +3838,7 @@
         <v>289</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>558</v>
+        <v>526</v>
       </c>
       <c r="D74" s="40"/>
       <c r="E74" s="41"/>
@@ -3930,7 +3852,7 @@
         <v>290</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>559</v>
+        <v>527</v>
       </c>
       <c r="D75" s="40"/>
       <c r="E75" s="41"/>
@@ -3944,7 +3866,7 @@
         <v>291</v>
       </c>
       <c r="C76" s="37" t="s">
-        <v>543</v>
+        <v>511</v>
       </c>
       <c r="D76" s="40"/>
       <c r="E76" s="41"/>
@@ -3970,7 +3892,7 @@
         <v>293</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>583</v>
+        <v>551</v>
       </c>
       <c r="D78" s="40"/>
       <c r="E78" s="41"/>
@@ -3984,7 +3906,7 @@
         <v>294</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>576</v>
+        <v>544</v>
       </c>
       <c r="D79" s="40"/>
       <c r="E79" s="41"/>
@@ -3998,7 +3920,7 @@
         <v>295</v>
       </c>
       <c r="C80" s="37" t="s">
-        <v>546</v>
+        <v>514</v>
       </c>
       <c r="D80" s="40"/>
       <c r="E80" s="41"/>
@@ -4012,7 +3934,7 @@
         <v>296</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>544</v>
+        <v>512</v>
       </c>
       <c r="D81" s="40"/>
       <c r="E81" s="41"/>
@@ -4026,7 +3948,7 @@
         <v>297</v>
       </c>
       <c r="C82" s="37" t="s">
-        <v>512</v>
+        <v>480</v>
       </c>
       <c r="D82" s="40"/>
       <c r="E82" s="41"/>
@@ -4040,7 +3962,7 @@
         <v>298</v>
       </c>
       <c r="C83" s="37" t="s">
-        <v>547</v>
+        <v>515</v>
       </c>
       <c r="D83" s="40"/>
       <c r="E83" s="41"/>
@@ -4054,7 +3976,7 @@
         <v>299</v>
       </c>
       <c r="C84" s="37" t="s">
-        <v>545</v>
+        <v>513</v>
       </c>
       <c r="D84" s="40"/>
       <c r="E84" s="41"/>
@@ -4068,7 +3990,7 @@
         <v>300</v>
       </c>
       <c r="C85" s="37" t="s">
-        <v>536</v>
+        <v>504</v>
       </c>
       <c r="D85" s="40"/>
       <c r="E85" s="41"/>
@@ -4082,7 +4004,7 @@
         <v>301</v>
       </c>
       <c r="C86" s="37" t="s">
-        <v>535</v>
+        <v>503</v>
       </c>
       <c r="D86" s="40"/>
       <c r="E86" s="41"/>
@@ -4096,7 +4018,7 @@
         <v>302</v>
       </c>
       <c r="C87" s="37" t="s">
-        <v>534</v>
+        <v>502</v>
       </c>
       <c r="D87" s="40"/>
       <c r="E87" s="41"/>
@@ -4110,7 +4032,7 @@
         <v>303</v>
       </c>
       <c r="C88" s="37" t="s">
-        <v>533</v>
+        <v>501</v>
       </c>
       <c r="D88" s="40"/>
       <c r="E88" s="41"/>
@@ -4124,7 +4046,7 @@
         <v>304</v>
       </c>
       <c r="C89" s="37" t="s">
-        <v>575</v>
+        <v>543</v>
       </c>
       <c r="D89" s="40"/>
       <c r="E89" s="41"/>
@@ -4137,9 +4059,7 @@
       <c r="B90" s="37" t="s">
         <v>305</v>
       </c>
-      <c r="C90" s="37" t="s">
-        <v>459</v>
-      </c>
+      <c r="C90" s="37"/>
       <c r="D90" s="40"/>
       <c r="E90" s="41"/>
       <c r="F90" s="43"/>
@@ -4151,9 +4071,7 @@
       <c r="B91" s="37" t="s">
         <v>306</v>
       </c>
-      <c r="C91" s="37" t="s">
-        <v>460</v>
-      </c>
+      <c r="C91" s="37"/>
       <c r="D91" s="40"/>
       <c r="E91" s="41"/>
       <c r="F91" s="43"/>
@@ -4165,9 +4083,7 @@
       <c r="B92" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="C92" s="37" t="s">
-        <v>461</v>
-      </c>
+      <c r="C92" s="37"/>
       <c r="D92" s="40"/>
       <c r="E92" s="41"/>
       <c r="F92" s="43"/>
@@ -4179,9 +4095,7 @@
       <c r="B93" s="37" t="s">
         <v>308</v>
       </c>
-      <c r="C93" s="37" t="s">
-        <v>462</v>
-      </c>
+      <c r="C93" s="37"/>
       <c r="D93" s="40"/>
       <c r="E93" s="41"/>
       <c r="F93" s="43"/>
@@ -4207,9 +4121,7 @@
       <c r="B95" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="C95" s="38" t="s">
-        <v>501</v>
-      </c>
+      <c r="C95" s="38"/>
       <c r="D95" s="40"/>
       <c r="E95" s="41"/>
       <c r="F95" s="43"/>
@@ -4221,9 +4133,7 @@
       <c r="B96" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="C96" s="38" t="s">
-        <v>505</v>
-      </c>
+      <c r="C96" s="38"/>
       <c r="D96" s="40"/>
       <c r="E96" s="41"/>
       <c r="F96" s="43"/>
@@ -4235,9 +4145,7 @@
       <c r="B97" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="C97" s="38" t="s">
-        <v>502</v>
-      </c>
+      <c r="C97" s="38"/>
       <c r="D97" s="40"/>
       <c r="E97" s="41"/>
       <c r="F97" s="43"/>
@@ -4249,9 +4157,7 @@
       <c r="B98" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="C98" s="38" t="s">
-        <v>503</v>
-      </c>
+      <c r="C98" s="38"/>
       <c r="D98" s="40"/>
       <c r="E98" s="41"/>
       <c r="F98" s="43"/>
@@ -4263,9 +4169,7 @@
       <c r="B99" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="C99" s="38" t="s">
-        <v>506</v>
-      </c>
+      <c r="C99" s="38"/>
       <c r="D99" s="40"/>
       <c r="E99" s="41"/>
       <c r="F99" s="43"/>
@@ -4277,9 +4181,7 @@
       <c r="B100" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="C100" s="38" t="s">
-        <v>507</v>
-      </c>
+      <c r="C100" s="38"/>
       <c r="D100" s="40"/>
       <c r="E100" s="41"/>
       <c r="F100" s="43"/>
@@ -4291,9 +4193,7 @@
       <c r="B101" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="C101" s="38" t="s">
-        <v>508</v>
-      </c>
+      <c r="C101" s="38"/>
       <c r="D101" s="40"/>
       <c r="E101" s="41"/>
       <c r="F101" s="43"/>
@@ -4305,9 +4205,7 @@
       <c r="B102" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="C102" s="38" t="s">
-        <v>509</v>
-      </c>
+      <c r="C102" s="38"/>
       <c r="D102" s="40"/>
       <c r="E102" s="41"/>
       <c r="F102" s="43"/>
@@ -4319,9 +4217,7 @@
       <c r="B103" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="C103" s="38" t="s">
-        <v>510</v>
-      </c>
+      <c r="C103" s="38"/>
       <c r="D103" s="40"/>
       <c r="E103" s="41"/>
       <c r="F103" s="43"/>
@@ -4333,9 +4229,7 @@
       <c r="B104" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="C104" s="38" t="s">
-        <v>511</v>
-      </c>
+      <c r="C104" s="38"/>
       <c r="D104" s="40"/>
       <c r="E104" s="41"/>
       <c r="F104" s="43"/>
@@ -4347,9 +4241,7 @@
       <c r="B105" s="37" t="s">
         <v>320</v>
       </c>
-      <c r="C105" s="37" t="s">
-        <v>463</v>
-      </c>
+      <c r="C105" s="37"/>
       <c r="D105" s="40"/>
       <c r="E105" s="41"/>
       <c r="F105" s="43"/>
@@ -4374,7 +4266,7 @@
         <v>322</v>
       </c>
       <c r="C107" s="37" t="s">
-        <v>584</v>
+        <v>552</v>
       </c>
       <c r="D107" s="40"/>
       <c r="E107" s="41"/>
@@ -4388,7 +4280,7 @@
         <v>323</v>
       </c>
       <c r="C108" s="37" t="s">
-        <v>582</v>
+        <v>550</v>
       </c>
       <c r="D108" s="40"/>
       <c r="E108" s="41"/>
@@ -4401,9 +4293,7 @@
       <c r="B109" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="C109" s="37" t="s">
-        <v>436</v>
-      </c>
+      <c r="C109" s="37"/>
       <c r="D109" s="40"/>
       <c r="E109" s="41"/>
       <c r="F109" s="43"/>
@@ -4415,9 +4305,7 @@
       <c r="B110" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="C110" s="37" t="s">
-        <v>464</v>
-      </c>
+      <c r="C110" s="37"/>
       <c r="D110" s="40"/>
       <c r="E110" s="41"/>
       <c r="F110" s="43"/>
@@ -4429,9 +4317,7 @@
       <c r="B111" s="37" t="s">
         <v>326</v>
       </c>
-      <c r="C111" s="37" t="s">
-        <v>465</v>
-      </c>
+      <c r="C111" s="37"/>
       <c r="D111" s="40"/>
       <c r="E111" s="41"/>
       <c r="F111" s="43"/>
@@ -4443,9 +4329,7 @@
       <c r="B112" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="C112" s="37" t="s">
-        <v>466</v>
-      </c>
+      <c r="C112" s="37"/>
       <c r="D112" s="40"/>
       <c r="E112" s="41"/>
       <c r="F112" s="43"/>
@@ -4457,9 +4341,7 @@
       <c r="B113" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="C113" s="37" t="s">
-        <v>467</v>
-      </c>
+      <c r="C113" s="37"/>
       <c r="D113" s="40"/>
       <c r="E113" s="41"/>
       <c r="F113" s="43"/>
@@ -4471,9 +4353,7 @@
       <c r="B114" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="C114" s="37" t="s">
-        <v>468</v>
-      </c>
+      <c r="C114" s="37"/>
       <c r="D114" s="40"/>
       <c r="E114" s="41"/>
       <c r="F114" s="43"/>
@@ -4485,9 +4365,7 @@
       <c r="B115" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="C115" s="37" t="s">
-        <v>469</v>
-      </c>
+      <c r="C115" s="37"/>
       <c r="D115" s="40"/>
       <c r="E115" s="41"/>
       <c r="F115" s="43"/>
@@ -4499,9 +4377,7 @@
       <c r="B116" s="37" t="s">
         <v>331</v>
       </c>
-      <c r="C116" s="37" t="s">
-        <v>470</v>
-      </c>
+      <c r="C116" s="37"/>
       <c r="D116" s="40"/>
       <c r="E116" s="41"/>
       <c r="F116" s="43"/>
@@ -4513,9 +4389,7 @@
       <c r="B117" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="C117" s="37" t="s">
-        <v>471</v>
-      </c>
+      <c r="C117" s="37"/>
       <c r="D117" s="40"/>
       <c r="E117" s="41"/>
       <c r="F117" s="43"/>
@@ -4527,9 +4401,7 @@
       <c r="B118" s="37" t="s">
         <v>333</v>
       </c>
-      <c r="C118" s="37" t="s">
-        <v>472</v>
-      </c>
+      <c r="C118" s="37"/>
       <c r="D118" s="40"/>
       <c r="E118" s="41"/>
       <c r="F118" s="43"/>
@@ -4541,9 +4413,7 @@
       <c r="B119" s="37" t="s">
         <v>334</v>
       </c>
-      <c r="C119" s="37" t="s">
-        <v>473</v>
-      </c>
+      <c r="C119" s="37"/>
       <c r="D119" s="40"/>
       <c r="E119" s="41"/>
       <c r="F119" s="43"/>
@@ -4555,9 +4425,7 @@
       <c r="B120" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="C120" s="37" t="s">
-        <v>474</v>
-      </c>
+      <c r="C120" s="37"/>
       <c r="D120" s="40"/>
       <c r="E120" s="41"/>
       <c r="F120" s="43"/>
@@ -4569,9 +4437,7 @@
       <c r="B121" s="37" t="s">
         <v>336</v>
       </c>
-      <c r="C121" s="37" t="s">
-        <v>475</v>
-      </c>
+      <c r="C121" s="37"/>
       <c r="D121" s="40"/>
       <c r="E121" s="41"/>
       <c r="F121" s="43"/>
@@ -4583,9 +4449,7 @@
       <c r="B122" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="C122" s="37" t="s">
-        <v>441</v>
-      </c>
+      <c r="C122" s="37"/>
       <c r="D122" s="40"/>
       <c r="E122" s="41"/>
       <c r="F122" s="43"/>
@@ -4597,9 +4461,7 @@
       <c r="B123" s="37" t="s">
         <v>338</v>
       </c>
-      <c r="C123" s="37" t="s">
-        <v>440</v>
-      </c>
+      <c r="C123" s="37"/>
       <c r="D123" s="40"/>
       <c r="E123" s="41"/>
       <c r="F123" s="43"/>
@@ -4611,9 +4473,7 @@
       <c r="B124" s="37" t="s">
         <v>339</v>
       </c>
-      <c r="C124" s="37" t="s">
-        <v>439</v>
-      </c>
+      <c r="C124" s="37"/>
       <c r="D124" s="40"/>
       <c r="E124" s="41"/>
       <c r="F124" s="43"/>
@@ -4625,9 +4485,7 @@
       <c r="B125" s="37" t="s">
         <v>340</v>
       </c>
-      <c r="C125" s="37" t="s">
-        <v>438</v>
-      </c>
+      <c r="C125" s="37"/>
       <c r="D125" s="40"/>
       <c r="E125" s="41"/>
       <c r="F125" s="43"/>
@@ -4639,9 +4497,7 @@
       <c r="B126" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="C126" s="37" t="s">
-        <v>437</v>
-      </c>
+      <c r="C126" s="37"/>
       <c r="D126" s="40"/>
       <c r="E126" s="41"/>
       <c r="F126" s="43"/>
@@ -4726,7 +4582,7 @@
         <v>348</v>
       </c>
       <c r="C133" s="37" t="s">
-        <v>562</v>
+        <v>530</v>
       </c>
       <c r="D133" s="40"/>
       <c r="E133" s="41"/>
@@ -4740,7 +4596,7 @@
         <v>349</v>
       </c>
       <c r="C134" s="37" t="s">
-        <v>561</v>
+        <v>529</v>
       </c>
       <c r="D134" s="40"/>
       <c r="E134" s="41"/>
@@ -4754,7 +4610,7 @@
         <v>350</v>
       </c>
       <c r="C135" s="37" t="s">
-        <v>560</v>
+        <v>528</v>
       </c>
       <c r="D135" s="40"/>
       <c r="E135" s="41"/>
@@ -4803,9 +4659,7 @@
       <c r="B139" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="C139" s="37" t="s">
-        <v>430</v>
-      </c>
+      <c r="C139" s="37"/>
       <c r="D139" s="40"/>
       <c r="E139" s="41"/>
       <c r="F139" s="43"/>
@@ -4817,9 +4671,7 @@
       <c r="B140" s="37" t="s">
         <v>355</v>
       </c>
-      <c r="C140" s="37" t="s">
-        <v>436</v>
-      </c>
+      <c r="C140" s="37"/>
       <c r="D140" s="40"/>
       <c r="E140" s="41"/>
       <c r="F140" s="43"/>
@@ -4829,7 +4681,7 @@
         <v>136</v>
       </c>
       <c r="B141" s="37" t="s">
-        <v>607</v>
+        <v>575</v>
       </c>
       <c r="C141" s="37"/>
       <c r="D141" s="40"/>
@@ -4841,7 +4693,7 @@
         <v>137</v>
       </c>
       <c r="B142" s="37" t="s">
-        <v>608</v>
+        <v>576</v>
       </c>
       <c r="C142" s="37"/>
       <c r="D142" s="40"/>
@@ -4853,7 +4705,7 @@
         <v>138</v>
       </c>
       <c r="B143" s="37" t="s">
-        <v>609</v>
+        <v>577</v>
       </c>
       <c r="C143" s="37"/>
       <c r="D143" s="40"/>
@@ -4865,7 +4717,7 @@
         <v>139</v>
       </c>
       <c r="B144" s="37" t="s">
-        <v>610</v>
+        <v>578</v>
       </c>
       <c r="C144" s="37"/>
       <c r="D144" s="40"/>
@@ -4877,7 +4729,7 @@
         <v>140</v>
       </c>
       <c r="B145" s="37" t="s">
-        <v>611</v>
+        <v>579</v>
       </c>
       <c r="C145" s="37"/>
       <c r="D145" s="40"/>
@@ -4889,7 +4741,7 @@
         <v>141</v>
       </c>
       <c r="B146" s="37" t="s">
-        <v>612</v>
+        <v>580</v>
       </c>
       <c r="C146" s="37"/>
       <c r="D146" s="40"/>
@@ -4937,7 +4789,7 @@
         <v>145</v>
       </c>
       <c r="B150" s="37" t="s">
-        <v>613</v>
+        <v>581</v>
       </c>
       <c r="C150" s="37"/>
       <c r="D150" s="40"/>
@@ -4949,7 +4801,7 @@
         <v>146</v>
       </c>
       <c r="B151" s="37" t="s">
-        <v>614</v>
+        <v>582</v>
       </c>
       <c r="C151" s="37"/>
       <c r="D151" s="40"/>
@@ -4961,7 +4813,7 @@
         <v>147</v>
       </c>
       <c r="B152" s="37" t="s">
-        <v>615</v>
+        <v>583</v>
       </c>
       <c r="C152" s="37"/>
       <c r="D152" s="40"/>
@@ -4973,7 +4825,7 @@
         <v>148</v>
       </c>
       <c r="B153" s="37" t="s">
-        <v>616</v>
+        <v>584</v>
       </c>
       <c r="C153" s="37"/>
       <c r="D153" s="40"/>
@@ -4985,7 +4837,7 @@
         <v>149</v>
       </c>
       <c r="B154" s="37" t="s">
-        <v>617</v>
+        <v>585</v>
       </c>
       <c r="C154" s="37"/>
       <c r="D154" s="40"/>
@@ -5275,9 +5127,7 @@
       <c r="B178" s="37" t="s">
         <v>382</v>
       </c>
-      <c r="C178" s="37" t="s">
-        <v>455</v>
-      </c>
+      <c r="C178" s="37"/>
       <c r="D178" s="40"/>
       <c r="E178" s="41"/>
       <c r="F178" s="43"/>
@@ -5289,9 +5139,7 @@
       <c r="B179" s="37" t="s">
         <v>383</v>
       </c>
-      <c r="C179" s="37" t="s">
-        <v>456</v>
-      </c>
+      <c r="C179" s="37"/>
       <c r="D179" s="40"/>
       <c r="E179" s="41"/>
       <c r="F179" s="43"/>
@@ -5303,9 +5151,7 @@
       <c r="B180" s="37" t="s">
         <v>384</v>
       </c>
-      <c r="C180" s="37" t="s">
-        <v>457</v>
-      </c>
+      <c r="C180" s="37"/>
       <c r="D180" s="40"/>
       <c r="E180" s="41"/>
       <c r="F180" s="43"/>
@@ -5317,9 +5163,7 @@
       <c r="B181" s="37" t="s">
         <v>385</v>
       </c>
-      <c r="C181" s="37" t="s">
-        <v>458</v>
-      </c>
+      <c r="C181" s="37"/>
       <c r="D181" s="40"/>
       <c r="E181" s="41"/>
       <c r="F181" s="43"/>
@@ -5439,9 +5283,7 @@
       <c r="B191" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="C191" s="37" t="s">
-        <v>454</v>
-      </c>
+      <c r="C191" s="37"/>
       <c r="D191" s="40"/>
       <c r="E191" s="41"/>
       <c r="F191" s="43"/>
@@ -5453,9 +5295,7 @@
       <c r="B192" s="37" t="s">
         <v>398</v>
       </c>
-      <c r="C192" s="37" t="s">
-        <v>442</v>
-      </c>
+      <c r="C192" s="37"/>
       <c r="D192" s="40"/>
       <c r="E192" s="41"/>
       <c r="F192" s="43"/>
@@ -5467,9 +5307,7 @@
       <c r="B193" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="C193" s="37" t="s">
-        <v>443</v>
-      </c>
+      <c r="C193" s="37"/>
       <c r="D193" s="40"/>
       <c r="E193" s="41"/>
       <c r="F193" s="43"/>
@@ -5481,9 +5319,7 @@
       <c r="B194" s="37" t="s">
         <v>400</v>
       </c>
-      <c r="C194" s="37" t="s">
-        <v>444</v>
-      </c>
+      <c r="C194" s="37"/>
       <c r="D194" s="40"/>
       <c r="E194" s="41"/>
       <c r="F194" s="43"/>
@@ -5495,9 +5331,7 @@
       <c r="B195" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="C195" s="37" t="s">
-        <v>445</v>
-      </c>
+      <c r="C195" s="37"/>
       <c r="D195" s="40"/>
       <c r="E195" s="41"/>
       <c r="F195" s="43"/>
@@ -5509,9 +5343,7 @@
       <c r="B196" s="37" t="s">
         <v>402</v>
       </c>
-      <c r="C196" s="37" t="s">
-        <v>446</v>
-      </c>
+      <c r="C196" s="37"/>
       <c r="D196" s="40"/>
       <c r="E196" s="41"/>
       <c r="F196" s="43"/>
@@ -5523,9 +5355,7 @@
       <c r="B197" s="37" t="s">
         <v>403</v>
       </c>
-      <c r="C197" s="37" t="s">
-        <v>447</v>
-      </c>
+      <c r="C197" s="37"/>
       <c r="D197" s="40"/>
       <c r="E197" s="41"/>
       <c r="F197" s="43"/>
@@ -5537,9 +5367,7 @@
       <c r="B198" s="37" t="s">
         <v>405</v>
       </c>
-      <c r="C198" s="37" t="s">
-        <v>448</v>
-      </c>
+      <c r="C198" s="37"/>
       <c r="D198" s="40"/>
       <c r="E198" s="41"/>
       <c r="F198" s="43"/>
@@ -5551,9 +5379,7 @@
       <c r="B199" s="37" t="s">
         <v>406</v>
       </c>
-      <c r="C199" s="37" t="s">
-        <v>449</v>
-      </c>
+      <c r="C199" s="37"/>
       <c r="D199" s="40"/>
       <c r="E199" s="41"/>
       <c r="F199" s="43"/>
@@ -5565,9 +5391,7 @@
       <c r="B200" s="37" t="s">
         <v>407</v>
       </c>
-      <c r="C200" s="37" t="s">
-        <v>450</v>
-      </c>
+      <c r="C200" s="37"/>
       <c r="D200" s="40"/>
       <c r="E200" s="41"/>
       <c r="F200" s="43"/>
@@ -5579,9 +5403,7 @@
       <c r="B201" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="C201" s="37" t="s">
-        <v>453</v>
-      </c>
+      <c r="C201" s="37"/>
       <c r="D201" s="40"/>
       <c r="E201" s="41"/>
       <c r="F201" s="43"/>
@@ -5593,9 +5415,7 @@
       <c r="B202" s="37" t="s">
         <v>409</v>
       </c>
-      <c r="C202" s="37" t="s">
-        <v>451</v>
-      </c>
+      <c r="C202" s="37"/>
       <c r="D202" s="40"/>
       <c r="E202" s="41"/>
       <c r="F202" s="43"/>
@@ -5607,9 +5427,7 @@
       <c r="B203" s="37" t="s">
         <v>410</v>
       </c>
-      <c r="C203" s="37" t="s">
-        <v>452</v>
-      </c>
+      <c r="C203" s="37"/>
       <c r="D203" s="40"/>
       <c r="E203" s="41"/>
       <c r="F203" s="43"/>
@@ -5811,7 +5629,7 @@
         <v>426</v>
       </c>
       <c r="B220" s="37" t="s">
-        <v>618</v>
+        <v>586</v>
       </c>
       <c r="C220" s="37"/>
       <c r="D220" s="40"/>
@@ -5823,7 +5641,7 @@
         <v>210</v>
       </c>
       <c r="B221" s="37" t="s">
-        <v>619</v>
+        <v>587</v>
       </c>
       <c r="C221" s="37"/>
       <c r="D221" s="40"/>
@@ -5835,7 +5653,7 @@
         <v>211</v>
       </c>
       <c r="B222" s="37" t="s">
-        <v>620</v>
+        <v>588</v>
       </c>
       <c r="C222" s="37"/>
       <c r="D222" s="40"/>
@@ -5847,9 +5665,8 @@
         <v>212</v>
       </c>
       <c r="B223" s="37" t="s">
-        <v>621</v>
-      </c>
-      <c r="C223" s="37"/>
+        <v>589</v>
+      </c>
       <c r="D223" s="40"/>
       <c r="E223" s="41"/>
       <c r="F223" s="43"/>
@@ -5859,7 +5676,7 @@
         <v>213</v>
       </c>
       <c r="B224" s="37" t="s">
-        <v>622</v>
+        <v>590</v>
       </c>
       <c r="C224" s="37"/>
       <c r="D224" s="40"/>
@@ -5871,7 +5688,7 @@
         <v>214</v>
       </c>
       <c r="B225" s="37" t="s">
-        <v>623</v>
+        <v>591</v>
       </c>
       <c r="C225" s="37"/>
       <c r="D225" s="40"/>
@@ -5883,7 +5700,7 @@
         <v>215</v>
       </c>
       <c r="B226" s="37" t="s">
-        <v>624</v>
+        <v>592</v>
       </c>
       <c r="C226" s="37"/>
       <c r="D226" s="40"/>
@@ -5895,7 +5712,7 @@
         <v>216</v>
       </c>
       <c r="B227" s="37" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="C227" s="37"/>
       <c r="D227" s="40"/>
@@ -5907,10 +5724,10 @@
         <v>217</v>
       </c>
       <c r="B228" s="37" t="s">
-        <v>626</v>
+        <v>594</v>
       </c>
       <c r="C228" s="37" t="s">
-        <v>647</v>
+        <v>615</v>
       </c>
       <c r="D228" s="40"/>
       <c r="E228" s="41"/>
@@ -5921,7 +5738,7 @@
         <v>218</v>
       </c>
       <c r="B229" s="37" t="s">
-        <v>627</v>
+        <v>595</v>
       </c>
       <c r="C229" s="37"/>
       <c r="D229" s="40"/>
@@ -5933,10 +5750,10 @@
         <v>219</v>
       </c>
       <c r="B230" s="37" t="s">
-        <v>628</v>
+        <v>596</v>
       </c>
       <c r="C230" s="37" t="s">
-        <v>578</v>
+        <v>546</v>
       </c>
       <c r="D230" s="40"/>
       <c r="E230" s="41"/>
@@ -5947,10 +5764,10 @@
         <v>220</v>
       </c>
       <c r="B231" s="37" t="s">
-        <v>629</v>
+        <v>597</v>
       </c>
       <c r="C231" s="37" t="s">
-        <v>577</v>
+        <v>545</v>
       </c>
       <c r="D231" s="40"/>
       <c r="E231" s="41"/>
@@ -5958,10 +5775,10 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="35" t="s">
-        <v>567</v>
+        <v>535</v>
       </c>
       <c r="B232" s="37" t="s">
-        <v>630</v>
+        <v>598</v>
       </c>
       <c r="C232" s="37"/>
       <c r="D232" s="40"/>
@@ -5970,10 +5787,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="35" t="s">
-        <v>568</v>
+        <v>536</v>
       </c>
       <c r="B233" s="37" t="s">
-        <v>631</v>
+        <v>599</v>
       </c>
       <c r="C233" s="37"/>
       <c r="D233" s="40"/>
@@ -5982,10 +5799,10 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="35" t="s">
-        <v>573</v>
+        <v>541</v>
       </c>
       <c r="B234" s="37" t="s">
-        <v>632</v>
+        <v>600</v>
       </c>
       <c r="C234" s="37"/>
       <c r="D234" s="40"/>
@@ -5994,10 +5811,10 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="35" t="s">
-        <v>569</v>
+        <v>537</v>
       </c>
       <c r="B235" s="37" t="s">
-        <v>633</v>
+        <v>601</v>
       </c>
       <c r="C235" s="37"/>
       <c r="D235" s="40"/>
@@ -6006,10 +5823,10 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="35" t="s">
-        <v>570</v>
+        <v>538</v>
       </c>
       <c r="B236" s="37" t="s">
-        <v>634</v>
+        <v>602</v>
       </c>
       <c r="C236" s="37"/>
       <c r="D236" s="40"/>
@@ -6018,13 +5835,13 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="35" t="s">
+        <v>516</v>
+      </c>
+      <c r="B237" s="37" t="s">
+        <v>603</v>
+      </c>
+      <c r="C237" s="37" t="s">
         <v>548</v>
-      </c>
-      <c r="B237" s="37" t="s">
-        <v>635</v>
-      </c>
-      <c r="C237" s="37" t="s">
-        <v>580</v>
       </c>
       <c r="D237" s="40"/>
       <c r="E237" s="41"/>
@@ -6032,13 +5849,13 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="35" t="s">
-        <v>549</v>
+        <v>517</v>
       </c>
       <c r="B238" s="37" t="s">
-        <v>636</v>
+        <v>604</v>
       </c>
       <c r="C238" s="37" t="s">
-        <v>579</v>
+        <v>547</v>
       </c>
       <c r="D238" s="40"/>
       <c r="E238" s="41"/>
@@ -6046,10 +5863,10 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="35" t="s">
-        <v>550</v>
+        <v>518</v>
       </c>
       <c r="B239" s="37" t="s">
-        <v>637</v>
+        <v>605</v>
       </c>
       <c r="C239" s="37"/>
       <c r="D239" s="40"/>
@@ -6058,10 +5875,10 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="35" t="s">
-        <v>551</v>
+        <v>519</v>
       </c>
       <c r="B240" s="37" t="s">
-        <v>566</v>
+        <v>534</v>
       </c>
       <c r="C240" s="37"/>
       <c r="D240" s="40"/>
@@ -6070,10 +5887,10 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="35" t="s">
-        <v>552</v>
+        <v>520</v>
       </c>
       <c r="B241" s="37" t="s">
-        <v>638</v>
+        <v>606</v>
       </c>
       <c r="C241" s="37"/>
       <c r="D241" s="40"/>
@@ -6082,10 +5899,10 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="35" t="s">
-        <v>553</v>
+        <v>521</v>
       </c>
       <c r="B242" s="37" t="s">
-        <v>639</v>
+        <v>607</v>
       </c>
       <c r="C242" s="37"/>
       <c r="D242" s="40"/>
@@ -6094,10 +5911,10 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="35" t="s">
-        <v>554</v>
+        <v>522</v>
       </c>
       <c r="B243" s="37" t="s">
-        <v>640</v>
+        <v>608</v>
       </c>
       <c r="C243" s="37"/>
       <c r="D243" s="40"/>
@@ -6106,13 +5923,13 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="35" t="s">
-        <v>555</v>
+        <v>523</v>
       </c>
       <c r="B244" s="37" t="s">
-        <v>641</v>
+        <v>609</v>
       </c>
       <c r="C244" s="37" t="s">
-        <v>581</v>
+        <v>549</v>
       </c>
       <c r="D244" s="40"/>
       <c r="E244" s="41"/>
@@ -6120,10 +5937,10 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="35" t="s">
-        <v>556</v>
+        <v>524</v>
       </c>
       <c r="B245" s="37" t="s">
-        <v>642</v>
+        <v>610</v>
       </c>
       <c r="C245" s="37"/>
       <c r="D245" s="40"/>
@@ -6132,13 +5949,13 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="35" t="s">
-        <v>571</v>
+        <v>539</v>
       </c>
       <c r="B246" s="37" t="s">
-        <v>643</v>
+        <v>611</v>
       </c>
       <c r="C246" s="37" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="D246" s="40"/>
       <c r="E246" s="41"/>
@@ -6146,10 +5963,10 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="35" t="s">
-        <v>572</v>
+        <v>540</v>
       </c>
       <c r="B247" s="37" t="s">
-        <v>644</v>
+        <v>612</v>
       </c>
       <c r="C247" s="37"/>
       <c r="D247" s="40"/>
@@ -6158,7 +5975,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="35" t="s">
-        <v>648</v>
+        <v>616</v>
       </c>
       <c r="B248" s="37" t="s">
         <v>2</v>
@@ -6172,7 +5989,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="35" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
       <c r="B249" s="37" t="s">
         <v>3</v>
@@ -6186,7 +6003,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="35" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="B250" s="37" t="s">
         <v>4</v>
@@ -6200,7 +6017,7 @@
     </row>
     <row r="251" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="36" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="B251" s="39" t="s">
         <v>5</v>
@@ -6222,8 +6039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F188CE91-FEB8-4BF7-A561-AE7C92FE4091}">
   <dimension ref="A1:BZ51"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2:BL5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6280,7 +6097,7 @@
       </c>
       <c r="M1" s="29"/>
       <c r="N1" s="21" t="s">
-        <v>588</v>
+        <v>556</v>
       </c>
       <c r="O1" s="22">
         <v>1</v>
@@ -6317,7 +6134,7 @@
       </c>
       <c r="Z1" s="29"/>
       <c r="AA1" s="21" t="s">
-        <v>596</v>
+        <v>564</v>
       </c>
       <c r="AB1" s="22">
         <v>1</v>
@@ -6354,7 +6171,7 @@
       </c>
       <c r="AM1" s="30"/>
       <c r="AN1" s="21" t="s">
-        <v>597</v>
+        <v>565</v>
       </c>
       <c r="AO1" s="22">
         <v>1</v>
@@ -6391,7 +6208,7 @@
       </c>
       <c r="AZ1" s="30"/>
       <c r="BA1" s="21" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="BB1" s="22">
         <v>1</v>
@@ -6428,7 +6245,7 @@
       </c>
       <c r="BM1" s="29"/>
       <c r="BN1" s="21" t="s">
-        <v>586</v>
+        <v>554</v>
       </c>
       <c r="BO1" s="22">
         <v>1</v>
@@ -6473,34 +6290,34 @@
         <v>428</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>492</v>
+        <v>470</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>497</v>
+        <v>475</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>482</v>
+        <v>460</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>493</v>
+        <v>471</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>495</v>
+        <v>473</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>496</v>
+        <v>474</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>490</v>
+        <v>468</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>491</v>
+        <v>469</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="24">
@@ -6738,13 +6555,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>539</v>
+        <v>507</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>476</v>
+        <v>454</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -6753,22 +6570,22 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>483</v>
+        <v>461</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>484</v>
+        <v>462</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>486</v>
+        <v>464</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>487</v>
+        <v>465</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>488</v>
+        <v>466</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>527</v>
+        <v>495</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="24">
@@ -7009,10 +6826,10 @@
         <v>433</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -7021,13 +6838,13 @@
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>481</v>
+        <v>459</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>489</v>
+        <v>467</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>533</v>
+        <v>501</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>427</v>
@@ -7272,7 +7089,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>431</v>
@@ -7281,22 +7098,22 @@
         <v>432</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>537</v>
+        <v>505</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>538</v>
+        <v>506</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>512</v>
+        <v>480</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>535</v>
+        <v>503</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>534</v>
+        <v>502</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>536</v>
+        <v>504</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>4</v>
@@ -7572,7 +7389,7 @@
       </c>
       <c r="M6" s="29"/>
       <c r="N6" s="21" t="s">
-        <v>602</v>
+        <v>570</v>
       </c>
       <c r="O6" s="22">
         <v>1</v>
@@ -7609,7 +7426,7 @@
       </c>
       <c r="Z6" s="29"/>
       <c r="AA6" s="21" t="s">
-        <v>592</v>
+        <v>560</v>
       </c>
       <c r="AB6" s="22">
         <v>1</v>
@@ -7646,7 +7463,7 @@
       </c>
       <c r="AM6" s="30"/>
       <c r="AN6" s="21" t="s">
-        <v>599</v>
+        <v>567</v>
       </c>
       <c r="AO6" s="22">
         <v>1</v>
@@ -7683,7 +7500,7 @@
       </c>
       <c r="AZ6" s="30"/>
       <c r="BA6" s="21" t="s">
-        <v>655</v>
+        <v>623</v>
       </c>
       <c r="BB6" s="22">
         <v>1</v>
@@ -7720,7 +7537,7 @@
       </c>
       <c r="BM6" s="29"/>
       <c r="BN6" s="26" t="s">
-        <v>587</v>
+        <v>555</v>
       </c>
       <c r="BO6" s="27">
         <v>1</v>
@@ -7762,37 +7579,37 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>581</v>
+        <v>549</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>542</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>504</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>513</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>574</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>455</v>
-      </c>
       <c r="H7" s="13" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>514</v>
+        <v>482</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>515</v>
-      </c>
-      <c r="K7" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="K7" s="50" t="s">
         <v>429</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>516</v>
+        <v>484</v>
       </c>
       <c r="M7" s="29"/>
       <c r="N7" s="24">
@@ -8004,11 +7821,11 @@
       </c>
       <c r="BR7" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="BS7" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="BT7" s="1">
         <f t="shared" si="0"/>
@@ -8016,7 +7833,7 @@
       </c>
       <c r="BU7" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="BV7" s="1">
         <f t="shared" si="0"/>
@@ -8031,8 +7848,8 @@
         <v>4</v>
       </c>
       <c r="BY7" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>AL7*1+AY7*2+AL12*4+AY12*8+AL17*16+AY17*32+AL22*64+AY22*128+AL2*256+AY2*512+BL2*1024+BL7*2048+BL12*4096+BL17*8192+BL22*16384</f>
+        <v>132</v>
       </c>
       <c r="BZ7" s="29"/>
     </row>
@@ -8041,14 +7858,14 @@
         <v>2</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>528</v>
+        <v>496</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -8056,9 +7873,9 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="L8" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="L8" s="52" t="s">
         <v>436</v>
       </c>
       <c r="M8" s="29"/>
@@ -8263,7 +8080,7 @@
       </c>
       <c r="BP8" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="BQ8" s="1">
         <f t="shared" si="1"/>
@@ -8271,7 +8088,7 @@
       </c>
       <c r="BR8" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="BS8" s="1">
         <f t="shared" si="1"/>
@@ -8283,7 +8100,7 @@
       </c>
       <c r="BU8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="BV8" s="1">
         <f t="shared" si="1"/>
@@ -8299,7 +8116,7 @@
       </c>
       <c r="BY8" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="BZ8" s="29"/>
     </row>
@@ -8311,28 +8128,28 @@
         <v>433</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>520</v>
+        <v>488</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>430</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>479</v>
+        <v>457</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>544</v>
+        <v>512</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>540</v>
+        <v>508</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>2</v>
@@ -8354,7 +8171,7 @@
       </c>
       <c r="Q9" s="1" t="str" cm="1">
         <f t="array" ref="Q9">_xlfn.XLOOKUP(D9,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D9,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D9,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D9,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0x63</v>
+        <v>0x36</v>
       </c>
       <c r="R9" s="1" t="str" cm="1">
         <f t="array" ref="R9">_xlfn.XLOOKUP(E9,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E9,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E9,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E9,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -8402,7 +8219,7 @@
       </c>
       <c r="AD9" s="1" cm="1">
         <f t="array" ref="AD9">IF(_xlfn.XLOOKUP(D9,KEYS!$D$1:$D$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!Q9,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="1" cm="1">
         <f t="array" ref="AE9">IF(_xlfn.XLOOKUP(E9,KEYS!$D$1:$D$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!R9,1,0)</f>
@@ -8544,7 +8361,7 @@
       </c>
       <c r="BQ9" s="1">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BR9" s="1">
         <f t="shared" si="2"/>
@@ -8585,7 +8402,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>431</v>
@@ -8594,22 +8411,22 @@
         <v>432</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>563</v>
+        <v>531</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>564</v>
+        <v>532</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>546</v>
+        <v>514</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>545</v>
+        <v>513</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>547</v>
+        <v>515</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>4</v>
@@ -8896,7 +8713,7 @@
       </c>
       <c r="M11" s="29"/>
       <c r="N11" s="21" t="s">
-        <v>589</v>
+        <v>557</v>
       </c>
       <c r="O11" s="22">
         <v>1</v>
@@ -8933,7 +8750,7 @@
       </c>
       <c r="Z11" s="29"/>
       <c r="AA11" s="21" t="s">
-        <v>593</v>
+        <v>561</v>
       </c>
       <c r="AB11" s="22">
         <v>1</v>
@@ -8970,7 +8787,7 @@
       </c>
       <c r="AM11" s="30"/>
       <c r="AN11" s="21" t="s">
-        <v>598</v>
+        <v>566</v>
       </c>
       <c r="AO11" s="22">
         <v>1</v>
@@ -9007,7 +8824,7 @@
       </c>
       <c r="AZ11" s="30"/>
       <c r="BA11" s="21" t="s">
-        <v>656</v>
+        <v>624</v>
       </c>
       <c r="BB11" s="22">
         <v>1</v>
@@ -9062,7 +8879,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>582</v>
+        <v>550</v>
       </c>
       <c r="C12" s="13">
         <v>1</v>
@@ -9091,7 +8908,7 @@
       <c r="K12" s="13">
         <v>9</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="51">
         <v>0</v>
       </c>
       <c r="M12" s="29"/>
@@ -9306,14 +9123,14 @@
         <v>2</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>575</v>
+        <v>543</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>517</v>
+        <v>485</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>523</v>
+        <v>491</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -9321,10 +9138,10 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>462</v>
+        <v>490</v>
+      </c>
+      <c r="L13" s="52" t="s">
+        <v>452</v>
       </c>
       <c r="M13" s="29"/>
       <c r="N13" s="24">
@@ -9372,7 +9189,7 @@
       </c>
       <c r="Y13" s="2" t="str" cm="1">
         <f t="array" ref="Y13">_xlfn.XLOOKUP(L13,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L13,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L13,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L13,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0x57</v>
+        <v>0x2E</v>
       </c>
       <c r="Z13" s="29"/>
       <c r="AA13" s="24">
@@ -9420,7 +9237,7 @@
       </c>
       <c r="AL13" s="2" cm="1">
         <f t="array" ref="AL13">IF(_xlfn.XLOOKUP(L13,KEYS!$D$1:$D$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!Y13,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM13" s="31"/>
       <c r="AN13" s="24">
@@ -9547,10 +9364,10 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="3" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>541</v>
+        <v>509</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>2</v>
@@ -9768,7 +9585,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>431</v>
@@ -9780,13 +9597,13 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="9" t="s">
-        <v>578</v>
+        <v>546</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>577</v>
+        <v>545</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>4</v>
@@ -10038,7 +9855,7 @@
       </c>
       <c r="M16" s="29"/>
       <c r="N16" s="21" t="s">
-        <v>590</v>
+        <v>558</v>
       </c>
       <c r="O16" s="22">
         <v>1</v>
@@ -10075,7 +9892,7 @@
       </c>
       <c r="Z16" s="29"/>
       <c r="AA16" s="21" t="s">
-        <v>594</v>
+        <v>562</v>
       </c>
       <c r="AB16" s="22">
         <v>1</v>
@@ -10112,7 +9929,7 @@
       </c>
       <c r="AM16" s="30"/>
       <c r="AN16" s="21" t="s">
-        <v>600</v>
+        <v>568</v>
       </c>
       <c r="AO16" s="22">
         <v>1</v>
@@ -10149,7 +9966,7 @@
       </c>
       <c r="AZ16" s="30"/>
       <c r="BA16" s="21" t="s">
-        <v>657</v>
+        <v>625</v>
       </c>
       <c r="BB16" s="22">
         <v>1</v>
@@ -10205,34 +10022,34 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="s">
-        <v>548</v>
+        <v>516</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>549</v>
+        <v>517</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>550</v>
+        <v>518</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>551</v>
+        <v>519</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>552</v>
+        <v>520</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>553</v>
+        <v>521</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>554</v>
+        <v>522</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>555</v>
+        <v>523</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>556</v>
+        <v>524</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>557</v>
+        <v>525</v>
       </c>
       <c r="M17" s="29"/>
       <c r="N17" s="24">
@@ -10446,31 +10263,31 @@
         <v>2</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>576</v>
+        <v>544</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>524</v>
+        <v>492</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>525</v>
+        <v>493</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>558</v>
+        <v>526</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>559</v>
+        <v>527</v>
       </c>
       <c r="M18" s="29"/>
       <c r="N18" s="24">
@@ -10482,7 +10299,7 @@
       </c>
       <c r="P18" s="1" t="str" cm="1">
         <f t="array" ref="P18">_xlfn.XLOOKUP(C18,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(C18,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(C18,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(C18,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xB8</v>
+        <v>0x21</v>
       </c>
       <c r="Q18" s="1" t="str" cm="1">
         <f t="array" ref="Q18">_xlfn.XLOOKUP(D18,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D18,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D18,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D18,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -10490,7 +10307,7 @@
       </c>
       <c r="R18" s="1" t="str" cm="1">
         <f t="array" ref="R18">_xlfn.XLOOKUP(E18,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E18,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E18,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E18,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xB9</v>
+        <v>0x2E</v>
       </c>
       <c r="S18" s="1" t="str" cm="1">
         <f t="array" ref="S18">_xlfn.XLOOKUP(F18,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F18,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F18,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F18,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -10502,7 +10319,7 @@
       </c>
       <c r="U18" s="1" t="str" cm="1">
         <f t="array" ref="U18">_xlfn.XLOOKUP(H18,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(H18,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(H18,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(H18,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xC4</v>
+        <v>0x34</v>
       </c>
       <c r="V18" s="1" t="str" cm="1">
         <f t="array" ref="V18">_xlfn.XLOOKUP(I18,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I18,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I18,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I18,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -10550,7 +10367,7 @@
       </c>
       <c r="AH18" s="1" cm="1">
         <f t="array" ref="AH18">IF(_xlfn.XLOOKUP(H18,KEYS!$D$1:$D$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!U18,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI18" s="1" cm="1">
         <f t="array" ref="AI18">IF(_xlfn.XLOOKUP(I18,KEYS!$D$1:$D$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!V18,1,0)</f>
@@ -10578,7 +10395,7 @@
       </c>
       <c r="AP18" s="1" cm="1">
         <f t="array" ref="AP18">IF(_xlfn.XLOOKUP(C18,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!P18,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ18" s="1" cm="1">
         <f t="array" ref="AQ18">IF(_xlfn.XLOOKUP(D18,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!Q18,1,0)</f>
@@ -10586,7 +10403,7 @@
       </c>
       <c r="AR18" s="1" cm="1">
         <f t="array" ref="AR18">IF(_xlfn.XLOOKUP(E18,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!R18,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS18" s="1" cm="1">
         <f t="array" ref="AS18">IF(_xlfn.XLOOKUP(F18,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!S18,1,0)</f>
@@ -10687,28 +10504,28 @@
         <v>433</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>521</v>
+        <v>489</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>530</v>
+        <v>498</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>529</v>
+        <v>497</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>526</v>
+        <v>494</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>647</v>
+        <v>615</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>542</v>
+        <v>510</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>2</v>
@@ -10924,7 +10741,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>431</v>
@@ -10933,18 +10750,18 @@
         <v>432</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="9" t="s">
-        <v>580</v>
+        <v>548</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>583</v>
+        <v>551</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>579</v>
+        <v>547</v>
       </c>
       <c r="K20" s="10" t="s">
         <v>4</v>
@@ -11194,7 +11011,7 @@
       </c>
       <c r="M21" s="29"/>
       <c r="N21" s="21" t="s">
-        <v>591</v>
+        <v>559</v>
       </c>
       <c r="O21" s="22">
         <v>1</v>
@@ -11231,7 +11048,7 @@
       </c>
       <c r="Z21" s="29"/>
       <c r="AA21" s="21" t="s">
-        <v>595</v>
+        <v>563</v>
       </c>
       <c r="AB21" s="22">
         <v>1</v>
@@ -11268,7 +11085,7 @@
       </c>
       <c r="AM21" s="30"/>
       <c r="AN21" s="21" t="s">
-        <v>601</v>
+        <v>569</v>
       </c>
       <c r="AO21" s="22">
         <v>1</v>
@@ -11305,7 +11122,7 @@
       </c>
       <c r="AZ21" s="30"/>
       <c r="BA21" s="21" t="s">
-        <v>658</v>
+        <v>626</v>
       </c>
       <c r="BB21" s="22">
         <v>1</v>
@@ -11364,31 +11181,31 @@
         <v>435</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>565</v>
+        <v>533</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>517</v>
+        <v>485</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>519</v>
+        <v>487</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>518</v>
+        <v>486</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>451</v>
+        <v>444</v>
+      </c>
+      <c r="L22" s="51" t="s">
+        <v>442</v>
       </c>
       <c r="M22" s="29"/>
       <c r="N22" s="24">
@@ -11408,11 +11225,11 @@
       </c>
       <c r="R22" s="13" t="str" cm="1">
         <f t="array" ref="R22">_xlfn.XLOOKUP(E22,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E22,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E22,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E22,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xCC</v>
+        <v>0x20</v>
       </c>
       <c r="S22" s="13" t="str" cm="1">
         <f t="array" ref="S22">_xlfn.XLOOKUP(F22,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F22,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F22,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F22,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xB8</v>
+        <v>0x21</v>
       </c>
       <c r="T22" s="13" t="str" cm="1">
         <f t="array" ref="T22">_xlfn.XLOOKUP(G22,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(G22,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(G22,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(G22,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -11420,7 +11237,7 @@
       </c>
       <c r="U22" s="13" t="str" cm="1">
         <f t="array" ref="U22">_xlfn.XLOOKUP(H22,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(H22,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(H22,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(H22,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xC9</v>
+        <v>0x23</v>
       </c>
       <c r="V22" s="13" t="str" cm="1">
         <f t="array" ref="V22">_xlfn.XLOOKUP(I22,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I22,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I22,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I22,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -11436,7 +11253,7 @@
       </c>
       <c r="Y22" s="14" t="str" cm="1">
         <f t="array" ref="Y22">_xlfn.XLOOKUP(L22,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L22,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L22,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L22,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xCE</v>
+        <v>0x27</v>
       </c>
       <c r="Z22" s="29"/>
       <c r="AA22" s="24">
@@ -11504,11 +11321,11 @@
       </c>
       <c r="AR22" s="13" cm="1">
         <f t="array" ref="AR22">IF(_xlfn.XLOOKUP(E22,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!R22,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS22" s="13" cm="1">
         <f t="array" ref="AS22">IF(_xlfn.XLOOKUP(F22,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!S22,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT22" s="13" cm="1">
         <f t="array" ref="AT22">IF(_xlfn.XLOOKUP(G22,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!T22,1,0)</f>
@@ -11516,7 +11333,7 @@
       </c>
       <c r="AU22" s="13" cm="1">
         <f t="array" ref="AU22">IF(_xlfn.XLOOKUP(H22,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!U22,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV22" s="13" cm="1">
         <f t="array" ref="AV22">IF(_xlfn.XLOOKUP(I22,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!V22,1,0)</f>
@@ -11532,7 +11349,7 @@
       </c>
       <c r="AY22" s="14" cm="1">
         <f t="array" ref="AY22">IF(_xlfn.XLOOKUP(L22,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!Y22,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ22" s="31"/>
       <c r="BA22" s="24">
@@ -11602,29 +11419,21 @@
         <v>2</v>
       </c>
       <c r="B23" s="15"/>
-      <c r="C23" s="1" t="s">
-        <v>443</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="E23" s="1" t="s">
         <v>444</v>
       </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="L23" s="52" t="s">
         <v>448</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>458</v>
       </c>
       <c r="M23" s="29"/>
       <c r="N23" s="24">
@@ -11636,7 +11445,7 @@
       </c>
       <c r="P23" s="1" t="str" cm="1">
         <f t="array" ref="P23">_xlfn.XLOOKUP(C23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(C23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(C23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(C23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xC5</v>
+        <v>0x00</v>
       </c>
       <c r="Q23" s="1" t="str" cm="1">
         <f t="array" ref="Q23">_xlfn.XLOOKUP(D23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(D23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -11644,7 +11453,7 @@
       </c>
       <c r="R23" s="1" t="str" cm="1">
         <f t="array" ref="R23">_xlfn.XLOOKUP(E23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(E23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xC6</v>
+        <v>0x00</v>
       </c>
       <c r="S23" s="1" t="str" cm="1">
         <f t="array" ref="S23">_xlfn.XLOOKUP(F23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(F23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -11660,11 +11469,11 @@
       </c>
       <c r="V23" s="1" t="str" cm="1">
         <f t="array" ref="V23">_xlfn.XLOOKUP(I23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(I23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xC8</v>
+        <v>0x00</v>
       </c>
       <c r="W23" s="1" t="str" cm="1">
         <f t="array" ref="W23">_xlfn.XLOOKUP(J23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(J23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(J23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(J23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xCA</v>
+        <v>0x00</v>
       </c>
       <c r="X23" s="1" t="str" cm="1">
         <f t="array" ref="X23">_xlfn.XLOOKUP(K23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(K23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(K23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(K23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
@@ -11672,7 +11481,7 @@
       </c>
       <c r="Y23" s="2" t="str" cm="1">
         <f t="array" ref="Y23">_xlfn.XLOOKUP(L23,KEYS!$C:$C,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L23,KEYS!$D:$D,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L23,KEYS!$E:$E,"0x"&amp;KEYS!$A:$A,_xlfn.XLOOKUP(L23,KEYS!$F:$F,"0x"&amp;KEYS!$A:$A))))</f>
-        <v>0xB9</v>
+        <v>0x2E</v>
       </c>
       <c r="Z23" s="29"/>
       <c r="AA23" s="24">
@@ -11768,7 +11577,7 @@
       </c>
       <c r="AY23" s="2" cm="1">
         <f t="array" ref="AY23">IF(_xlfn.XLOOKUP(L23,KEYS!$E$1:$E$247,"0x"&amp;KEYS!$A$1:$A$247,0)=LAYERS!Y23,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ23" s="31"/>
       <c r="BA23" s="24">
@@ -11847,10 +11656,10 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="3" t="s">
-        <v>561</v>
+        <v>529</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>543</v>
+        <v>511</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>2</v>
@@ -12066,7 +11875,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>585</v>
+        <v>553</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>431</v>
@@ -12078,13 +11887,13 @@
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="9" t="s">
-        <v>562</v>
+        <v>530</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>560</v>
+        <v>528</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>584</v>
+        <v>552</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>4</v>
@@ -14376,6 +14185,36 @@
       <c r="BZ51" s="29"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="BO2:BY5">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB2:BL5 BB7:BL10 BB12:BL15 BB17:BL20 BB22:BL25 BO2:BY5 AO2:AY5 AO7:AY10 AO12:AY15 AO17:AY20 AO22:AY25 AB22:AL25 AB17:AL20 AB12:AL15 AB7:AL10 AB2:AL5">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO7:BY10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -14385,8 +14224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ACA031D-C442-44FE-A68E-C17CB201DDE1}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14818,7 +14657,7 @@
       </c>
       <c r="D9" s="1" t="str">
         <f>LAYERS!Q9&amp;","</f>
-        <v>0x63,</v>
+        <v>0x36,</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>LAYERS!R9&amp;","</f>
@@ -15054,7 +14893,7 @@
       </c>
       <c r="L13" s="2" t="str">
         <f>LAYERS!Y13&amp;","</f>
-        <v>0x57,</v>
+        <v>0x2E,</v>
       </c>
       <c r="M13" s="29"/>
     </row>
@@ -15273,7 +15112,7 @@
       </c>
       <c r="C18" s="1" t="str">
         <f>LAYERS!P18&amp;","</f>
-        <v>0xB8,</v>
+        <v>0x21,</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>LAYERS!Q18&amp;","</f>
@@ -15281,7 +15120,7 @@
       </c>
       <c r="E18" s="1" t="str">
         <f>LAYERS!R18&amp;","</f>
-        <v>0xB9,</v>
+        <v>0x2E,</v>
       </c>
       <c r="F18" s="1" t="str">
         <f>LAYERS!S18&amp;","</f>
@@ -15293,7 +15132,7 @@
       </c>
       <c r="H18" s="1" t="str">
         <f>LAYERS!U18&amp;","</f>
-        <v>0xC4,</v>
+        <v>0x34,</v>
       </c>
       <c r="I18" s="1" t="str">
         <f>LAYERS!V18&amp;","</f>
@@ -15485,11 +15324,11 @@
       </c>
       <c r="E22" s="13" t="str">
         <f>LAYERS!R22&amp;","</f>
-        <v>0xCC,</v>
+        <v>0x20,</v>
       </c>
       <c r="F22" s="13" t="str">
         <f>LAYERS!S22&amp;","</f>
-        <v>0xB8,</v>
+        <v>0x21,</v>
       </c>
       <c r="G22" s="13" t="str">
         <f>LAYERS!T22&amp;","</f>
@@ -15497,7 +15336,7 @@
       </c>
       <c r="H22" s="13" t="str">
         <f>LAYERS!U22&amp;","</f>
-        <v>0xC9,</v>
+        <v>0x23,</v>
       </c>
       <c r="I22" s="13" t="str">
         <f>LAYERS!V22&amp;","</f>
@@ -15513,7 +15352,7 @@
       </c>
       <c r="L22" s="14" t="str">
         <f>LAYERS!Y22&amp;","</f>
-        <v>0xCE,</v>
+        <v>0x27,</v>
       </c>
       <c r="M22" s="29"/>
     </row>
@@ -15528,7 +15367,7 @@
       </c>
       <c r="C23" s="1" t="str">
         <f>LAYERS!P23&amp;","</f>
-        <v>0xC5,</v>
+        <v>0x00,</v>
       </c>
       <c r="D23" s="1" t="str">
         <f>LAYERS!Q23&amp;","</f>
@@ -15536,7 +15375,7 @@
       </c>
       <c r="E23" s="1" t="str">
         <f>LAYERS!R23&amp;","</f>
-        <v>0xC6,</v>
+        <v>0x00,</v>
       </c>
       <c r="F23" s="1" t="str">
         <f>LAYERS!S23&amp;","</f>
@@ -15552,11 +15391,11 @@
       </c>
       <c r="I23" s="1" t="str">
         <f>LAYERS!V23&amp;","</f>
-        <v>0xC8,</v>
+        <v>0x00,</v>
       </c>
       <c r="J23" s="1" t="str">
         <f>LAYERS!W23&amp;","</f>
-        <v>0xCA,</v>
+        <v>0x00,</v>
       </c>
       <c r="K23" s="1" t="str">
         <f>LAYERS!X23&amp;","</f>
@@ -15564,7 +15403,7 @@
       </c>
       <c r="L23" s="2" t="str">
         <f>LAYERS!Y23&amp;","</f>
-        <v>0xB9,</v>
+        <v>0x2E,</v>
       </c>
       <c r="M23" s="29"/>
     </row>
@@ -15995,11 +15834,11 @@
       </c>
       <c r="E32" s="13" t="str">
         <f>LAYERS!BR7&amp;","</f>
-        <v>4,</v>
+        <v>132,</v>
       </c>
       <c r="F32" s="13" t="str">
         <f>LAYERS!BS7&amp;","</f>
-        <v>4,</v>
+        <v>132,</v>
       </c>
       <c r="G32" s="13" t="str">
         <f>LAYERS!BT7&amp;","</f>
@@ -16007,7 +15846,7 @@
       </c>
       <c r="H32" s="13" t="str">
         <f>LAYERS!BU7&amp;","</f>
-        <v>4,</v>
+        <v>132,</v>
       </c>
       <c r="I32" s="13" t="str">
         <f>LAYERS!BV7&amp;","</f>
@@ -16023,7 +15862,7 @@
       </c>
       <c r="L32" s="14" t="str">
         <f>LAYERS!BY7&amp;","</f>
-        <v>4,</v>
+        <v>132,</v>
       </c>
       <c r="M32" s="29"/>
     </row>
@@ -16038,7 +15877,7 @@
       </c>
       <c r="C33" s="1" t="str">
         <f>LAYERS!BP8&amp;","</f>
-        <v>8,</v>
+        <v>40,</v>
       </c>
       <c r="D33" s="1" t="str">
         <f>LAYERS!BQ8&amp;","</f>
@@ -16046,7 +15885,7 @@
       </c>
       <c r="E33" s="1" t="str">
         <f>LAYERS!BR8&amp;","</f>
-        <v>8,</v>
+        <v>40,</v>
       </c>
       <c r="F33" s="1" t="str">
         <f>LAYERS!BS8&amp;","</f>
@@ -16058,7 +15897,7 @@
       </c>
       <c r="H33" s="1" t="str">
         <f>LAYERS!BU8&amp;","</f>
-        <v>0,</v>
+        <v>16,</v>
       </c>
       <c r="I33" s="1" t="str">
         <f>LAYERS!BV8&amp;","</f>
@@ -16074,7 +15913,7 @@
       </c>
       <c r="L33" s="2" t="str">
         <f>LAYERS!BY8&amp;","</f>
-        <v>0,</v>
+        <v>132,</v>
       </c>
       <c r="M33" s="29"/>
     </row>
@@ -16093,7 +15932,7 @@
       </c>
       <c r="D34" s="1" t="str">
         <f>LAYERS!BQ9&amp;","</f>
-        <v>16,</v>
+        <v>17,</v>
       </c>
       <c r="E34" s="1" t="str">
         <f>LAYERS!BR9&amp;","</f>

</xml_diff>